<commit_message>
decompression script now in python and uses similar GUI to the trace analysis script
</commit_message>
<xml_diff>
--- a/analysis/scripts/trace_analysis/processed-.xlsx
+++ b/analysis/scripts/trace_analysis/processed-.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="184">
   <si>
     <t>Trace</t>
   </si>
@@ -37,280 +37,529 @@
     <t>1</t>
   </si>
   <si>
-    <t>18251</t>
+    <t>42145</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1544459837426393148</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>1544459837426409997</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>1544459837426437375</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1544459837426442910</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>42135</t>
+  </si>
+  <si>
+    <t>1544459837426475070</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1544459837426476344</t>
+  </si>
+  <si>
+    <t>42136</t>
+  </si>
+  <si>
+    <t>1544459837426516483</t>
+  </si>
+  <si>
+    <t>42134</t>
+  </si>
+  <si>
+    <t>1544459837426519705</t>
+  </si>
+  <si>
+    <t>1544459837426521844</t>
+  </si>
+  <si>
+    <t>1544459837426531777</t>
+  </si>
+  <si>
+    <t>42138</t>
+  </si>
+  <si>
+    <t>1544459837426547901</t>
+  </si>
+  <si>
+    <t>1544459837426548947</t>
+  </si>
+  <si>
+    <t>42137</t>
+  </si>
+  <si>
+    <t>1544459837426557018</t>
+  </si>
+  <si>
+    <t>1544459837426559154</t>
+  </si>
+  <si>
+    <t>42141</t>
+  </si>
+  <si>
+    <t>1544459837426559428</t>
+  </si>
+  <si>
+    <t>1544459837426560422</t>
+  </si>
+  <si>
+    <t>42140</t>
+  </si>
+  <si>
+    <t>1544459837426570449</t>
+  </si>
+  <si>
+    <t>1544459837426571639</t>
+  </si>
+  <si>
+    <t>42139</t>
+  </si>
+  <si>
+    <t>1544459837426580175</t>
+  </si>
+  <si>
+    <t>1544459837426582374</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1544459837426604816</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>1544459837426632856</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>1544459837426636035</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>1544459837426636476</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>1544459837426637777</t>
+  </si>
+  <si>
+    <t>42148</t>
+  </si>
+  <si>
+    <t>1544459837779374216</t>
+  </si>
+  <si>
+    <t>1544459837779382015</t>
+  </si>
+  <si>
+    <t>1544459837779389345</t>
+  </si>
+  <si>
+    <t>1544459837779392064</t>
+  </si>
+  <si>
+    <t>1544459837779436280</t>
+  </si>
+  <si>
+    <t>1544459837779439382</t>
+  </si>
+  <si>
+    <t>1544459837779456590</t>
+  </si>
+  <si>
+    <t>1544459837779466184</t>
+  </si>
+  <si>
+    <t>1544459837779468746</t>
+  </si>
+  <si>
+    <t>1544459837779469676</t>
+  </si>
+  <si>
+    <t>1544459837779470986</t>
+  </si>
+  <si>
+    <t>1544459837779475440</t>
+  </si>
+  <si>
+    <t>1544459837779476289</t>
+  </si>
+  <si>
+    <t>1544459837779476483</t>
+  </si>
+  <si>
+    <t>1544459837779480564</t>
+  </si>
+  <si>
+    <t>1544459837779483714</t>
+  </si>
+  <si>
+    <t>1544459837779488931</t>
+  </si>
+  <si>
+    <t>1544459837779490037</t>
+  </si>
+  <si>
+    <t>1544459837779493343</t>
+  </si>
+  <si>
+    <t>1544459837779494367</t>
+  </si>
+  <si>
+    <t>1544459837779524330</t>
+  </si>
+  <si>
+    <t>1544459837779531042</t>
+  </si>
+  <si>
+    <t>1544459837779531931</t>
+  </si>
+  <si>
+    <t>1544459837779532345</t>
+  </si>
+  <si>
+    <t>1544459837779533848</t>
+  </si>
+  <si>
+    <t>42142</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>1544088821582866164</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>1544088821582924614</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>18241</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1544088821582932698</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>1544088821582933946</t>
-  </si>
-  <si>
-    <t>18242</t>
+    <t>1544459838061897461</t>
+  </si>
+  <si>
+    <t>1544459838061905839</t>
+  </si>
+  <si>
+    <t>1544459838061931063</t>
+  </si>
+  <si>
+    <t>1544459838061936210</t>
+  </si>
+  <si>
+    <t>1544459838061996406</t>
+  </si>
+  <si>
+    <t>1544459838061999756</t>
+  </si>
+  <si>
+    <t>1544459838062003270</t>
+  </si>
+  <si>
+    <t>1544459838062005026</t>
+  </si>
+  <si>
+    <t>1544459838062019349</t>
+  </si>
+  <si>
+    <t>1544459838062021626</t>
+  </si>
+  <si>
+    <t>1544459838062022611</t>
+  </si>
+  <si>
+    <t>1544459838062024759</t>
+  </si>
+  <si>
+    <t>1544459838062028241</t>
+  </si>
+  <si>
+    <t>1544459838062030457</t>
+  </si>
+  <si>
+    <t>1544459838062064190</t>
+  </si>
+  <si>
+    <t>1544459838062067813</t>
+  </si>
+  <si>
+    <t>1544459838062075235</t>
+  </si>
+  <si>
+    <t>1544459838062078033</t>
+  </si>
+  <si>
+    <t>1544459838062088156</t>
+  </si>
+  <si>
+    <t>1544459838062090625</t>
+  </si>
+  <si>
+    <t>1544459838062170277</t>
+  </si>
+  <si>
+    <t>1544459838062177940</t>
+  </si>
+  <si>
+    <t>1544459838062178770</t>
+  </si>
+  <si>
+    <t>1544459838062179177</t>
+  </si>
+  <si>
+    <t>1544459838062180828</t>
+  </si>
+  <si>
+    <t>42146</t>
+  </si>
+  <si>
+    <t>1544459838389662857</t>
+  </si>
+  <si>
+    <t>1544459838389669643</t>
+  </si>
+  <si>
+    <t>1544459838389676700</t>
+  </si>
+  <si>
+    <t>1544459838389679395</t>
+  </si>
+  <si>
+    <t>1544459838389716517</t>
+  </si>
+  <si>
+    <t>1544459838389718765</t>
+  </si>
+  <si>
+    <t>1544459838389729752</t>
+  </si>
+  <si>
+    <t>1544459838389732162</t>
+  </si>
+  <si>
+    <t>1544459838389741675</t>
+  </si>
+  <si>
+    <t>1544459838389742885</t>
+  </si>
+  <si>
+    <t>1544459838389773795</t>
+  </si>
+  <si>
+    <t>1544459838389776129</t>
+  </si>
+  <si>
+    <t>1544459838389794043</t>
+  </si>
+  <si>
+    <t>1544459838389796865</t>
+  </si>
+  <si>
+    <t>1544459838389798172</t>
+  </si>
+  <si>
+    <t>1544459838389798923</t>
+  </si>
+  <si>
+    <t>1544459838389800380</t>
+  </si>
+  <si>
+    <t>1544459838389811902</t>
+  </si>
+  <si>
+    <t>1544459838389820347</t>
+  </si>
+  <si>
+    <t>1544459838389823038</t>
+  </si>
+  <si>
+    <t>1544459838389894125</t>
+  </si>
+  <si>
+    <t>1544459838389900763</t>
+  </si>
+  <si>
+    <t>1544459838389901510</t>
+  </si>
+  <si>
+    <t>1544459838389901851</t>
+  </si>
+  <si>
+    <t>1544459838389902985</t>
+  </si>
+  <si>
+    <t>1544459838563332769</t>
+  </si>
+  <si>
+    <t>1544459838563342582</t>
+  </si>
+  <si>
+    <t>1544459838563352601</t>
+  </si>
+  <si>
+    <t>1544459838563357249</t>
+  </si>
+  <si>
+    <t>1544459838563443298</t>
+  </si>
+  <si>
+    <t>1544459838563446281</t>
+  </si>
+  <si>
+    <t>1544459838563447612</t>
+  </si>
+  <si>
+    <t>1544459838563449259</t>
+  </si>
+  <si>
+    <t>1544459838563451335</t>
+  </si>
+  <si>
+    <t>1544459838563474326</t>
+  </si>
+  <si>
+    <t>1544459838563486625</t>
+  </si>
+  <si>
+    <t>1544459838563487850</t>
+  </si>
+  <si>
+    <t>1544459838563503582</t>
+  </si>
+  <si>
+    <t>1544459838563505295</t>
+  </si>
+  <si>
+    <t>1544459838563507494</t>
+  </si>
+  <si>
+    <t>1544459838563509289</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>1544088821582936669</t>
-  </si>
-  <si>
-    <t>1544088821582937934</t>
-  </si>
-  <si>
-    <t>18243</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>1544088821582938223</t>
-  </si>
-  <si>
-    <t>1544088821582939377</t>
-  </si>
-  <si>
-    <t>18244</t>
-  </si>
-  <si>
-    <t>1544088821582939917</t>
-  </si>
-  <si>
-    <t>1544088821582941890</t>
-  </si>
-  <si>
-    <t>18245</t>
-  </si>
-  <si>
-    <t>1544088821582949296</t>
-  </si>
-  <si>
-    <t>1544088821582950055</t>
-  </si>
-  <si>
-    <t>18247</t>
-  </si>
-  <si>
-    <t>1544088821582957401</t>
-  </si>
-  <si>
-    <t>1544088821582958133</t>
-  </si>
-  <si>
-    <t>18248</t>
-  </si>
-  <si>
-    <t>1544088821582960481</t>
-  </si>
-  <si>
-    <t>1544088821582961019</t>
-  </si>
-  <si>
-    <t>18246</t>
-  </si>
-  <si>
-    <t>1544088821582962842</t>
-  </si>
-  <si>
-    <t>1544088821582963383</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>1544088821582967038</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>1544088821582984363</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>1544088821582986627</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>1544088821582986955</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>1544088821582987811</t>
-  </si>
-  <si>
-    <t>18253</t>
-  </si>
-  <si>
-    <t>1544088823421574553</t>
-  </si>
-  <si>
-    <t>1544088823421591607</t>
-  </si>
-  <si>
-    <t>1544088823421612397</t>
-  </si>
-  <si>
-    <t>1544088823421613199</t>
-  </si>
-  <si>
-    <t>1544088823421625599</t>
-  </si>
-  <si>
-    <t>1544088823421628175</t>
-  </si>
-  <si>
-    <t>1544088823421629379</t>
-  </si>
-  <si>
-    <t>1544088823421630441</t>
-  </si>
-  <si>
-    <t>1544088823421631485</t>
-  </si>
-  <si>
-    <t>1544088823421633229</t>
-  </si>
-  <si>
-    <t>1544088823421633648</t>
-  </si>
-  <si>
-    <t>1544088823421633819</t>
-  </si>
-  <si>
-    <t>1544088823421634901</t>
-  </si>
-  <si>
-    <t>1544088823421636178</t>
-  </si>
-  <si>
-    <t>1544088823421636920</t>
-  </si>
-  <si>
-    <t>1544088823421639314</t>
-  </si>
-  <si>
-    <t>1544088823421640297</t>
-  </si>
-  <si>
-    <t>1544088823421641861</t>
-  </si>
-  <si>
-    <t>1544088823421647295</t>
-  </si>
-  <si>
-    <t>1544088823421653312</t>
-  </si>
-  <si>
-    <t>1544088823421654108</t>
-  </si>
-  <si>
-    <t>1544088823421654538</t>
-  </si>
-  <si>
-    <t>1544088823421655520</t>
-  </si>
-  <si>
-    <t>18249</t>
-  </si>
-  <si>
-    <t>1544088824960487710</t>
-  </si>
-  <si>
-    <t>1544088824960502390</t>
-  </si>
-  <si>
-    <t>1544088824960507916</t>
-  </si>
-  <si>
-    <t>1544088824960508853</t>
-  </si>
-  <si>
-    <t>1544088824960511530</t>
-  </si>
-  <si>
-    <t>1544088824960513507</t>
-  </si>
-  <si>
-    <t>1544088824960514655</t>
-  </si>
-  <si>
-    <t>1544088824960516102</t>
-  </si>
-  <si>
-    <t>1544088824960516298</t>
-  </si>
-  <si>
-    <t>1544088824960517243</t>
-  </si>
-  <si>
-    <t>1544088824960520251</t>
-  </si>
-  <si>
-    <t>1544088824960520973</t>
-  </si>
-  <si>
-    <t>1544088824960521174</t>
-  </si>
-  <si>
-    <t>1544088824960521733</t>
-  </si>
-  <si>
-    <t>1544088824960522215</t>
-  </si>
-  <si>
-    <t>1544088824960523066</t>
-  </si>
-  <si>
-    <t>1544088824960525639</t>
-  </si>
-  <si>
-    <t>1544088824960526162</t>
-  </si>
-  <si>
-    <t>1544088824960528981</t>
-  </si>
-  <si>
-    <t>1544088824960533422</t>
-  </si>
-  <si>
-    <t>1544088824960534076</t>
-  </si>
-  <si>
-    <t>1544088824960534369</t>
-  </si>
-  <si>
-    <t>1544088824960535160</t>
+    <t>1544459838563786377</t>
+  </si>
+  <si>
+    <t>1544459838563790759</t>
+  </si>
+  <si>
+    <t>1544459838563839525</t>
+  </si>
+  <si>
+    <t>1544459838563841063</t>
+  </si>
+  <si>
+    <t>1544459838563941502</t>
+  </si>
+  <si>
+    <t>1544459838563959168</t>
+  </si>
+  <si>
+    <t>1544459838563960533</t>
+  </si>
+  <si>
+    <t>1544459838563960874</t>
+  </si>
+  <si>
+    <t>1544459838563964894</t>
+  </si>
+  <si>
+    <t>1544459838775900790</t>
+  </si>
+  <si>
+    <t>1544459838775908524</t>
+  </si>
+  <si>
+    <t>1544459838775916087</t>
+  </si>
+  <si>
+    <t>1544459838775919063</t>
+  </si>
+  <si>
+    <t>1544459838775990142</t>
+  </si>
+  <si>
+    <t>1544459838775993362</t>
+  </si>
+  <si>
+    <t>1544459838775997311</t>
+  </si>
+  <si>
+    <t>1544459838776001431</t>
+  </si>
+  <si>
+    <t>1544459838776002830</t>
+  </si>
+  <si>
+    <t>1544459838776016520</t>
+  </si>
+  <si>
+    <t>1544459838776017428</t>
+  </si>
+  <si>
+    <t>1544459838776019097</t>
+  </si>
+  <si>
+    <t>1544459838776020171</t>
+  </si>
+  <si>
+    <t>1544459838776022496</t>
+  </si>
+  <si>
+    <t>1544459838776027255</t>
+  </si>
+  <si>
+    <t>1544459838776028156</t>
+  </si>
+  <si>
+    <t>1544459838776037162</t>
+  </si>
+  <si>
+    <t>1544459838776039388</t>
+  </si>
+  <si>
+    <t>1544459838776064133</t>
+  </si>
+  <si>
+    <t>1544459838776066612</t>
+  </si>
+  <si>
+    <t>1544459838776102345</t>
+  </si>
+  <si>
+    <t>1544459838776112333</t>
+  </si>
+  <si>
+    <t>1544459838776113295</t>
+  </si>
+  <si>
+    <t>1544459838776113913</t>
+  </si>
+  <si>
+    <t>1544459838776115436</t>
   </si>
   <si>
     <t>Trace ID analytics</t>
@@ -343,11 +592,11 @@
     <font>
       <color rgb="FF777777"/>
     </font>
+    <font/>
     <font>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
     </font>
-    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -378,22 +627,22 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
     <cellStyle hidden="0" name="Title" xfId="1"/>
     <cellStyle hidden="0" name="Description" xfId="2"/>
-    <cellStyle hidden="0" name="Header" xfId="3"/>
-    <cellStyle hidden="0" name="Row" xfId="4"/>
+    <cellStyle hidden="0" name="Row" xfId="3"/>
+    <cellStyle hidden="0" name="Header" xfId="4"/>
     <cellStyle hidden="0" name="Row, integer" xfId="5"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -401,8 +650,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="regular_trace_entries" headerRowCount="1" id="1" name="regular_trace_entries" ref="A2:D71">
-  <autoFilter ref="A2:D71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="regular_trace_entries" headerRowCount="1" id="1" name="regular_trace_entries" ref="A2:D152">
+  <autoFilter ref="A2:D152"/>
   <tableColumns count="4">
     <tableColumn id="1" name="traceId"/>
     <tableColumn id="2" name="cpuId"/>
@@ -714,7 +963,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
@@ -782,69 +1031,69 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -852,279 +1101,279 @@
         <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1132,27 +1381,27 @@
         <v>11</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1160,27 +1409,27 @@
         <v>15</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1188,41 +1437,41 @@
         <v>15</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1230,234 +1479,234 @@
         <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>79</v>
@@ -1465,13 +1714,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>80</v>
@@ -1482,10 +1731,10 @@
         <v>11</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>81</v>
@@ -1493,13 +1742,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>82</v>
@@ -1507,13 +1756,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>83</v>
@@ -1521,13 +1770,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>84</v>
@@ -1535,13 +1784,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>85</v>
@@ -1549,10 +1798,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>13</v>
@@ -1566,10 +1815,10 @@
         <v>15</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>87</v>
@@ -1580,10 +1829,10 @@
         <v>15</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>88</v>
@@ -1591,13 +1840,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>89</v>
@@ -1605,13 +1854,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>90</v>
@@ -1619,13 +1868,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>91</v>
@@ -1633,13 +1882,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>92</v>
@@ -1647,13 +1896,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>93</v>
@@ -1661,13 +1910,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>94</v>
@@ -1675,13 +1924,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="3" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>95</v>
@@ -1689,13 +1938,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="3" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>96</v>
@@ -1703,16 +1952,1150 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1751,15 +3134,15 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>99</v>
+        <v>182</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>100</v>
+        <v>183</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>

</xml_diff>